<commit_message>
add monthly water use script
</commit_message>
<xml_diff>
--- a/ml_experiments/annual_v_0_0/features_status.xlsx
+++ b/ml_experiments/annual_v_0_0/features_status.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\water_use\ml_experiments\annual_v_0_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\water_use\CAWSC_WaterUse\ml_experiments\annual_v_0_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803B3FCB-2871-4111-B5ED-620350F3538C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFAA7E3-27DA-4456-91CF-7CFB399CC5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="annual" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="286">
   <si>
     <t>is_swud</t>
   </si>
@@ -847,24 +847,6 @@
     <t>pop</t>
   </si>
   <si>
-    <t>aggregation method</t>
-  </si>
-  <si>
-    <t>sum</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>mode</t>
-  </si>
-  <si>
-    <t>NAN</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
     <t>sample_id</t>
   </si>
   <si>
@@ -872,6 +854,48 @@
   </si>
   <si>
     <t>System Identifier</t>
+  </si>
+  <si>
+    <t>cii_frac</t>
+  </si>
+  <si>
+    <t>Fraction of water use for irrigation and industrial sectors</t>
+  </si>
+  <si>
+    <t>dom_frac</t>
+  </si>
+  <si>
+    <t>fraction of domestic water use</t>
+  </si>
+  <si>
+    <t>is_thermal</t>
+  </si>
+  <si>
+    <t>Flag indicating using public water for a thermoelectric  power.</t>
+  </si>
+  <si>
+    <t>monthly Skip</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>simil_stat</t>
+  </si>
+  <si>
+    <t>monthly_fraction</t>
+  </si>
+  <si>
+    <t>Metric that measures similiarity to temperature seasonality</t>
+  </si>
+  <si>
+    <t>Monthly fraction</t>
+  </si>
+  <si>
+    <t>monthly_wu</t>
+  </si>
+  <si>
+    <t>Monthly water use</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1473,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1625,7 +1649,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1947,11 +1970,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O136"/>
+  <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A139" sqref="A139:XFD140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,12 +1987,10 @@
     <col min="6" max="6" width="25.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1"/>
-    <col min="10" max="10" width="24" style="5" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>108</v>
       </c>
@@ -1995,24 +2016,18 @@
         <v>141</v>
       </c>
       <c r="I1" s="64" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="J1" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="64" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>275</v>
-      </c>
       <c r="B2" s="20" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D2" s="20">
         <v>1</v>
@@ -2023,11 +2038,8 @@
       <c r="H2" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-    </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -2046,14 +2058,11 @@
       <c r="H3" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65" t="str">
-        <f>A3</f>
-        <v>is_swud</v>
-      </c>
-      <c r="K3" s="65"/>
-    </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
@@ -2074,18 +2083,11 @@
       <c r="H4" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I4" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="J4" s="65" t="str">
-        <f t="shared" ref="J4:J67" si="0">A4</f>
-        <v>population</v>
-      </c>
-      <c r="K4" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
         <v>268</v>
       </c>
@@ -2098,18 +2100,8 @@
       <c r="H5" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I5" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="J5" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>pop</v>
-      </c>
-      <c r="K5" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
@@ -2128,18 +2120,11 @@
       <c r="H6" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I6" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="J6" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>households2</v>
-      </c>
-      <c r="K6" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
@@ -2160,18 +2145,8 @@
       <c r="H7" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I7" s="65" t="s">
-        <v>271</v>
-      </c>
-      <c r="J7" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>pop_density</v>
-      </c>
-      <c r="K7" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>78</v>
       </c>
@@ -2188,18 +2163,8 @@
       <c r="H8" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I8" s="65" t="s">
-        <v>271</v>
-      </c>
-      <c r="J8" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>pop_house_ratio</v>
-      </c>
-      <c r="K8" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>79</v>
       </c>
@@ -2216,18 +2181,8 @@
       <c r="H9" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I9" s="65" t="s">
-        <v>271</v>
-      </c>
-      <c r="J9" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>family_size</v>
-      </c>
-      <c r="K9" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>81</v>
       </c>
@@ -2244,18 +2199,8 @@
       <c r="H10" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I10" s="65" t="s">
-        <v>271</v>
-      </c>
-      <c r="J10" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>county_tot_pop_2010</v>
-      </c>
-      <c r="K10" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>74</v>
       </c>
@@ -2272,18 +2217,8 @@
       <c r="H11" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="65" t="s">
-        <v>271</v>
-      </c>
-      <c r="J11" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>awuds_pop_cnt</v>
-      </c>
-      <c r="K11" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>77</v>
       </c>
@@ -2302,18 +2237,8 @@
       <c r="H12" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="I12" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="J12" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>n_houses</v>
-      </c>
-      <c r="K12" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>20</v>
       </c>
@@ -2332,18 +2257,11 @@
       <c r="H13" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J13" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>h_age_newer_2005</v>
-      </c>
-      <c r="K13" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
@@ -2362,18 +2280,11 @@
       <c r="H14" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J14" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>h_age_2000_2004</v>
-      </c>
-      <c r="K14" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
@@ -2392,18 +2303,11 @@
       <c r="H15" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J15" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>h_age_1990_1999</v>
-      </c>
-      <c r="K15" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
@@ -2422,18 +2326,11 @@
       <c r="H16" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J16" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>h_age_1980_1989</v>
-      </c>
-      <c r="K16" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
@@ -2452,19 +2349,12 @@
       <c r="H17" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J17" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>h_age_1970_1979</v>
-      </c>
-      <c r="K17" s="65">
-        <v>0</v>
-      </c>
-      <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>25</v>
       </c>
@@ -2483,19 +2373,12 @@
       <c r="H18" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J18" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>h_age_1960_1969</v>
-      </c>
-      <c r="K18" s="65">
-        <v>0</v>
-      </c>
-      <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>26</v>
       </c>
@@ -2514,18 +2397,11 @@
       <c r="H19" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J19" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>h_age_1950_1959</v>
-      </c>
-      <c r="K19" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>27</v>
       </c>
@@ -2544,18 +2420,11 @@
       <c r="H20" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J20" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>h_age_1940_1949</v>
-      </c>
-      <c r="K20" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>28</v>
       </c>
@@ -2574,18 +2443,11 @@
       <c r="H21" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J21" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>h_age_older_1939</v>
-      </c>
-      <c r="K21" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>29</v>
       </c>
@@ -2604,18 +2466,8 @@
       <c r="H22" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J22" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>median_h_year</v>
-      </c>
-      <c r="K22" s="65">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="s">
         <v>231</v>
       </c>
@@ -2634,18 +2486,8 @@
       <c r="H23" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J23" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>av_house_age</v>
-      </c>
-      <c r="K23" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
         <v>211</v>
       </c>
@@ -2664,18 +2506,8 @@
       <c r="H24" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I24" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J24" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>zill_nhouse</v>
-      </c>
-      <c r="K24" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>212</v>
       </c>
@@ -2694,18 +2526,8 @@
       <c r="H25" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J25" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>LotSizeSquareFeet_sum</v>
-      </c>
-      <c r="K25" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
         <v>214</v>
       </c>
@@ -2722,18 +2544,8 @@
       <c r="H26" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J26" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>YearBuilt_mean</v>
-      </c>
-      <c r="K26" s="65">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="s">
         <v>216</v>
       </c>
@@ -2750,18 +2562,8 @@
       <c r="H27" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J27" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>BuildingAreaSqFt_sum</v>
-      </c>
-      <c r="K27" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
         <v>220</v>
       </c>
@@ -2780,18 +2582,8 @@
       <c r="H28" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I28" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J28" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>NoOfStories_mean</v>
-      </c>
-      <c r="K28" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="s">
         <v>222</v>
       </c>
@@ -2810,18 +2602,8 @@
       <c r="H29" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J29" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>bdg_ftp_count</v>
-      </c>
-      <c r="K29" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="60" t="s">
         <v>223</v>
       </c>
@@ -2840,18 +2622,8 @@
       <c r="H30" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I30" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J30" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>bdg_gt_2median</v>
-      </c>
-      <c r="K30" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="60" t="s">
         <v>224</v>
       </c>
@@ -2870,18 +2642,8 @@
       <c r="H31" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I31" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J31" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>bdg_gt_4median</v>
-      </c>
-      <c r="K31" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>225</v>
       </c>
@@ -2900,18 +2662,8 @@
       <c r="H32" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I32" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J32" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>bdg_lt_2median</v>
-      </c>
-      <c r="K32" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="5" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" s="5" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="61" t="s">
         <v>226</v>
       </c>
@@ -2930,18 +2682,8 @@
       <c r="H33" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="I33" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J33" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>bdg_lt_4median</v>
-      </c>
-      <c r="K33" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:9" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>3</v>
       </c>
@@ -2960,18 +2702,11 @@
       <c r="H34" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I34" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J34" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_lt_10k</v>
-      </c>
-      <c r="K34" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>4</v>
       </c>
@@ -2990,18 +2725,11 @@
       <c r="H35" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I35" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J35" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_10K_15k</v>
-      </c>
-      <c r="K35" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>5</v>
       </c>
@@ -3020,18 +2748,11 @@
       <c r="H36" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I36" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J36" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_15k_20k</v>
-      </c>
-      <c r="K36" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
         <v>6</v>
       </c>
@@ -3050,18 +2771,11 @@
       <c r="H37" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I37" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J37" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_20k_25k</v>
-      </c>
-      <c r="K37" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>7</v>
       </c>
@@ -3080,18 +2794,11 @@
       <c r="H38" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I38" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J38" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_25k_30k</v>
-      </c>
-      <c r="K38" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>8</v>
       </c>
@@ -3110,18 +2817,11 @@
       <c r="H39" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I39" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J39" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_30k_35k</v>
-      </c>
-      <c r="K39" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>9</v>
       </c>
@@ -3140,18 +2840,11 @@
       <c r="H40" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I40" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J40" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_35k_40k</v>
-      </c>
-      <c r="K40" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>10</v>
       </c>
@@ -3170,18 +2863,11 @@
       <c r="H41" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I41" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J41" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_40k_45k</v>
-      </c>
-      <c r="K41" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>11</v>
       </c>
@@ -3200,18 +2886,11 @@
       <c r="H42" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I42" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J42" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_45k_50k</v>
-      </c>
-      <c r="K42" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>12</v>
       </c>
@@ -3230,18 +2909,11 @@
       <c r="H43" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I43" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J43" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_50k_60k</v>
-      </c>
-      <c r="K43" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>13</v>
       </c>
@@ -3260,18 +2932,11 @@
       <c r="H44" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I44" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J44" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_60k_75k</v>
-      </c>
-      <c r="K44" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>14</v>
       </c>
@@ -3290,18 +2955,11 @@
       <c r="H45" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I45" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J45" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_75k_100k</v>
-      </c>
-      <c r="K45" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>15</v>
       </c>
@@ -3320,18 +2978,11 @@
       <c r="H46" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I46" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J46" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_100k_125k</v>
-      </c>
-      <c r="K46" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>16</v>
       </c>
@@ -3350,18 +3001,11 @@
       <c r="H47" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I47" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J47" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_125k_150k</v>
-      </c>
-      <c r="K47" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
         <v>17</v>
       </c>
@@ -3380,18 +3024,11 @@
       <c r="H48" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I48" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J48" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_150k_200k</v>
-      </c>
-      <c r="K48" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>18</v>
       </c>
@@ -3410,18 +3047,11 @@
       <c r="H49" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I49" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J49" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_gt_200k</v>
-      </c>
-      <c r="K49" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>19</v>
       </c>
@@ -3440,18 +3070,8 @@
       <c r="H50" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I50" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J50" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>median_income</v>
-      </c>
-      <c r="K50" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>234</v>
       </c>
@@ -3466,18 +3086,8 @@
       <c r="H51" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I51" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J51" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>average_income</v>
-      </c>
-      <c r="K51" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>86</v>
       </c>
@@ -3494,18 +3104,8 @@
       <c r="H52" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I52" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J52" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>pov_2019</v>
-      </c>
-      <c r="K52" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>182</v>
       </c>
@@ -3524,18 +3124,8 @@
       <c r="H53" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I53" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J53" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>gini</v>
-      </c>
-      <c r="K53" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>30</v>
       </c>
@@ -3554,18 +3144,8 @@
       <c r="H54" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I54" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J54" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_employed</v>
-      </c>
-      <c r="K54" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>31</v>
       </c>
@@ -3584,18 +3164,8 @@
       <c r="H55" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I55" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J55" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_occupation</v>
-      </c>
-      <c r="K55" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>32</v>
       </c>
@@ -3614,18 +3184,8 @@
       <c r="H56" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I56" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J56" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_occ_management</v>
-      </c>
-      <c r="K56" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
         <v>33</v>
       </c>
@@ -3644,18 +3204,8 @@
       <c r="H57" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I57" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J57" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_occ_service</v>
-      </c>
-      <c r="K57" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>34</v>
       </c>
@@ -3674,18 +3224,8 @@
       <c r="H58" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I58" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J58" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_occ_sales_office</v>
-      </c>
-      <c r="K58" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="23" t="s">
         <v>35</v>
       </c>
@@ -3704,18 +3244,8 @@
       <c r="H59" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I59" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J59" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_occ_farm_fish_forest</v>
-      </c>
-      <c r="K59" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
         <v>36</v>
       </c>
@@ -3734,18 +3264,8 @@
       <c r="H60" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I60" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J60" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_occ_const_maint_repair</v>
-      </c>
-      <c r="K60" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="23" t="s">
         <v>37</v>
       </c>
@@ -3764,18 +3284,8 @@
       <c r="H61" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I61" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J61" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_occ_prod_trans_material</v>
-      </c>
-      <c r="K61" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="23" t="s">
         <v>87</v>
       </c>
@@ -3792,18 +3302,8 @@
       <c r="H62" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I62" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J62" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>income_cnty</v>
-      </c>
-      <c r="K62" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="23" t="s">
         <v>88</v>
       </c>
@@ -3820,18 +3320,8 @@
       <c r="H63" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I63" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J63" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_jobs_cnty</v>
-      </c>
-      <c r="K63" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="23" t="s">
         <v>89</v>
       </c>
@@ -3848,18 +3338,8 @@
       <c r="H64" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I64" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J64" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>indus_cnty</v>
-      </c>
-      <c r="K64" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
         <v>38</v>
       </c>
@@ -3878,18 +3358,8 @@
       <c r="H65" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I65" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J65" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_industry</v>
-      </c>
-      <c r="K65" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="23" t="s">
         <v>39</v>
       </c>
@@ -3908,18 +3378,8 @@
       <c r="H66" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I66" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J66" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_ind_ag_forest_fish_mining</v>
-      </c>
-      <c r="K66" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="23" t="s">
         <v>40</v>
       </c>
@@ -3938,18 +3398,8 @@
       <c r="H67" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I67" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J67" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>n_ind_construction</v>
-      </c>
-      <c r="K67" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="23" t="s">
         <v>41</v>
       </c>
@@ -3968,18 +3418,8 @@
       <c r="H68" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I68" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J68" s="6" t="str">
-        <f t="shared" ref="J68:J131" si="1">A68</f>
-        <v>n_ind_manufacturing</v>
-      </c>
-      <c r="K68" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="23" t="s">
         <v>42</v>
       </c>
@@ -3998,18 +3438,8 @@
       <c r="H69" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I69" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J69" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_wholesale_trade</v>
-      </c>
-      <c r="K69" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="23" t="s">
         <v>43</v>
       </c>
@@ -4028,18 +3458,8 @@
       <c r="H70" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I70" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J70" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_retail_trade</v>
-      </c>
-      <c r="K70" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="23" t="s">
         <v>44</v>
       </c>
@@ -4058,18 +3478,8 @@
       <c r="H71" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I71" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J71" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_trans_warehouse_utilities</v>
-      </c>
-      <c r="K71" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="23" t="s">
         <v>45</v>
       </c>
@@ -4088,18 +3498,8 @@
       <c r="H72" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I72" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J72" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_information</v>
-      </c>
-      <c r="K72" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="23" t="s">
         <v>46</v>
       </c>
@@ -4118,18 +3518,8 @@
       <c r="H73" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I73" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J73" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_finance</v>
-      </c>
-      <c r="K73" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="23" t="s">
         <v>47</v>
       </c>
@@ -4148,18 +3538,8 @@
       <c r="H74" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I74" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J74" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_prof_sci_admin_waste</v>
-      </c>
-      <c r="K74" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="23" t="s">
         <v>48</v>
       </c>
@@ -4178,18 +3558,8 @@
       <c r="H75" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I75" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J75" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_education_healthcare</v>
-      </c>
-      <c r="K75" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="23" t="s">
         <v>49</v>
       </c>
@@ -4208,18 +3578,8 @@
       <c r="H76" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I76" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J76" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_arts_entertain_foodservice</v>
-      </c>
-      <c r="K76" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
         <v>50</v>
       </c>
@@ -4238,18 +3598,8 @@
       <c r="H77" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I77" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J77" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_other</v>
-      </c>
-      <c r="K77" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="23" t="s">
         <v>51</v>
       </c>
@@ -4268,18 +3618,8 @@
       <c r="H78" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I78" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J78" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>n_ind_publicadmin</v>
-      </c>
-      <c r="K78" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="23" t="s">
         <v>104</v>
       </c>
@@ -4296,18 +3636,8 @@
       <c r="H79" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I79" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J79" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Num_establishments_2012</v>
-      </c>
-      <c r="K79" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
         <v>91</v>
       </c>
@@ -4322,18 +3652,8 @@
       <c r="H80" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I80" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J80" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>unemployment_cnty</v>
-      </c>
-      <c r="K80" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
         <v>105</v>
       </c>
@@ -4350,18 +3670,8 @@
       <c r="H81" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I81" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J81" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Num_establishments_2017</v>
-      </c>
-      <c r="K81" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="23" t="s">
         <v>218</v>
       </c>
@@ -4378,18 +3688,8 @@
       <c r="H82" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I82" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J82" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>TaxAmount_mean</v>
-      </c>
-      <c r="K82" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="23" t="s">
         <v>82</v>
       </c>
@@ -4408,18 +3708,11 @@
       <c r="H83" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I83" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J83" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_hschool</v>
-      </c>
-      <c r="K83" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
         <v>83</v>
       </c>
@@ -4438,18 +3731,11 @@
       <c r="H84" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I84" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J84" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_diploma</v>
-      </c>
-      <c r="K84" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="23" t="s">
         <v>84</v>
       </c>
@@ -4468,18 +3754,11 @@
       <c r="H85" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I85" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J85" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_college</v>
-      </c>
-      <c r="K85" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="25" t="s">
         <v>85</v>
       </c>
@@ -4498,18 +3777,11 @@
       <c r="H86" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="I86" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J86" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_high_edu</v>
-      </c>
-      <c r="K86" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>261</v>
       </c>
@@ -4519,18 +3791,8 @@
       <c r="H87" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I87" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J87" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_n_lt_ninth_gr</v>
-      </c>
-      <c r="K87" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>262</v>
       </c>
@@ -4540,18 +3802,8 @@
       <c r="H88" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I88" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J88" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_n_ninth_to_twelth_gr</v>
-      </c>
-      <c r="K88" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>263</v>
       </c>
@@ -4561,18 +3813,8 @@
       <c r="H89" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I89" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J89" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_n_hs_grad</v>
-      </c>
-      <c r="K89" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>264</v>
       </c>
@@ -4582,18 +3824,8 @@
       <c r="H90" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I90" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J90" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_n_some_college</v>
-      </c>
-      <c r="K90" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>265</v>
       </c>
@@ -4603,18 +3835,8 @@
       <c r="H91" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I91" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J91" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_n_associates</v>
-      </c>
-      <c r="K91" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>266</v>
       </c>
@@ -4624,18 +3846,8 @@
       <c r="H92" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I92" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J92" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_n_bachelors</v>
-      </c>
-      <c r="K92" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>267</v>
       </c>
@@ -4645,18 +3857,8 @@
       <c r="H93" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="I93" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J93" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>prc_n_masters_phd</v>
-      </c>
-      <c r="K93" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="27" t="s">
         <v>53</v>
       </c>
@@ -4675,15 +3877,11 @@
       <c r="H94" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="I94" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J94" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>etr_warm</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I94" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29" t="s">
         <v>54</v>
       </c>
@@ -4702,15 +3900,11 @@
       <c r="H95" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I95" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J95" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>etr_cool</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I95" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
         <v>55</v>
       </c>
@@ -4729,15 +3923,8 @@
       <c r="H96" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I96" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J96" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>etr</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29" t="s">
         <v>56</v>
       </c>
@@ -4756,15 +3943,11 @@
       <c r="H97" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I97" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J97" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pr_warm</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I97" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="29" t="s">
         <v>57</v>
       </c>
@@ -4783,15 +3966,11 @@
       <c r="H98" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I98" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J98" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pr_cool</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I98" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="29" t="s">
         <v>58</v>
       </c>
@@ -4810,15 +3989,8 @@
       <c r="H99" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I99" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J99" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pr</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
         <v>188</v>
       </c>
@@ -4837,15 +4009,8 @@
       <c r="H100" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I100" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J100" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pr_cumdev</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="29" t="s">
         <v>59</v>
       </c>
@@ -4864,15 +4029,11 @@
       <c r="H101" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I101" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J101" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>tmmn_warm</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I101" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
         <v>60</v>
       </c>
@@ -4891,15 +4052,11 @@
       <c r="H102" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I102" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J102" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>tmmn_cool</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I102" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29" t="s">
         <v>61</v>
       </c>
@@ -4918,15 +4075,8 @@
       <c r="H103" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I103" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J103" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>tmmn</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29" t="s">
         <v>62</v>
       </c>
@@ -4945,15 +4095,11 @@
       <c r="H104" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I104" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J104" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>tmmx_warm</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I104" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="29" t="s">
         <v>63</v>
       </c>
@@ -4972,15 +4118,11 @@
       <c r="H105" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I105" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J105" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>tmmx_cool</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I105" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29" t="s">
         <v>64</v>
       </c>
@@ -4999,15 +4141,8 @@
       <c r="H106" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I106" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J106" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>tmmx</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="29" t="s">
         <v>191</v>
       </c>
@@ -5028,22 +4163,17 @@
       <c r="H107" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I107" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J107" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>ardity_index</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="32" t="s">
         <v>107</v>
       </c>
       <c r="B108" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="C108" s="33"/>
+      <c r="C108" s="30" t="s">
+        <v>120</v>
+      </c>
       <c r="D108" s="33"/>
       <c r="E108" s="33"/>
       <c r="F108" s="33"/>
@@ -5053,18 +4183,11 @@
       <c r="H108" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="I108" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="J108" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>KG_climate_zone</v>
-      </c>
-      <c r="L108" t="s">
+      <c r="J108" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="34" t="s">
         <v>66</v>
       </c>
@@ -5081,15 +4204,8 @@
       <c r="H109" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="I109" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J109" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>LAT</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="36" t="s">
         <v>67</v>
       </c>
@@ -5106,15 +4222,8 @@
       <c r="H110" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="I110" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J110" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="36" t="s">
         <v>200</v>
       </c>
@@ -5133,15 +4242,11 @@
       <c r="H111" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="I111" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J111" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I111" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="36" t="s">
         <v>201</v>
       </c>
@@ -5160,15 +4265,11 @@
       <c r="H112" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="I112" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J112" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Y</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I112" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="36" t="s">
         <v>70</v>
       </c>
@@ -5185,15 +4286,8 @@
       <c r="H113" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="I113" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="J113" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>HUC2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="36" t="s">
         <v>80</v>
       </c>
@@ -5214,15 +4308,11 @@
       <c r="H114" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="I114" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="J114" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>fips</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="36" t="s">
         <v>71</v>
       </c>
@@ -5241,15 +4331,8 @@
       <c r="H115" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="I115" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="J115" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>county_id</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="36" t="s">
         <v>106</v>
       </c>
@@ -5266,15 +4349,8 @@
       <c r="H116" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="I116" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="J116" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>state_id</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="36" t="s">
         <v>92</v>
       </c>
@@ -5291,15 +4367,8 @@
       <c r="H117" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="I117" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J117" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>WSA_SQKM</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="38" t="s">
         <v>90</v>
       </c>
@@ -5313,18 +4382,11 @@
       <c r="E118" s="39"/>
       <c r="F118" s="39"/>
       <c r="G118" s="39"/>
-      <c r="H118" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="I118" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="J118" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>rur_urb_cnty</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="H118" s="37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="40" t="s">
         <v>65</v>
       </c>
@@ -5345,15 +4407,8 @@
       <c r="H119" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="I119" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="J119" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>sys_id</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="42" t="s">
         <v>75</v>
       </c>
@@ -5372,15 +4427,11 @@
       <c r="H120" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="I120" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="J120" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Ecode</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I120" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="44" t="s">
         <v>76</v>
       </c>
@@ -5397,15 +4448,8 @@
       <c r="H121" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="I121" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="J121" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Ecode_num</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="46" t="s">
         <v>93</v>
       </c>
@@ -5422,15 +4466,8 @@
       <c r="H122" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="I122" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J122" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Commercial</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="48" t="s">
         <v>94</v>
       </c>
@@ -5447,15 +4484,8 @@
       <c r="H123" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I123" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J123" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Conservation</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="48" t="s">
         <v>95</v>
       </c>
@@ -5472,15 +4502,8 @@
       <c r="H124" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I124" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J124" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Domestic</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="48" t="s">
         <v>96</v>
       </c>
@@ -5497,15 +4520,8 @@
       <c r="H125" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I125" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J125" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Industrial</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="48" t="s">
         <v>97</v>
       </c>
@@ -5522,15 +4538,8 @@
       <c r="H126" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I126" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J126" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Institutional</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="48" t="s">
         <v>98</v>
       </c>
@@ -5547,15 +4556,8 @@
       <c r="H127" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I127" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J127" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Recreation_Misc</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="48" t="s">
         <v>99</v>
       </c>
@@ -5572,15 +4574,8 @@
       <c r="H128" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I128" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J128" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Urban_Misc</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="48" t="s">
         <v>100</v>
       </c>
@@ -5597,15 +4592,8 @@
       <c r="H129" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I129" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J129" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Production</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="48" t="s">
         <v>101</v>
       </c>
@@ -5622,15 +4610,8 @@
       <c r="H130" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I130" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J130" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Urban_Parks</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="48" t="s">
         <v>102</v>
       </c>
@@ -5647,15 +4628,8 @@
       <c r="H131" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I131" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J131" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Water</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="50" t="s">
         <v>103</v>
       </c>
@@ -5674,112 +4648,226 @@
       <c r="H132" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="I132" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J132" s="6" t="str">
-        <f t="shared" ref="J132:J136" si="2">A132</f>
-        <v>NoData</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A133" s="52" t="s">
+      <c r="I132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B133" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="C133" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="D133" s="55"/>
+      <c r="E133" s="55"/>
+      <c r="F133" s="55"/>
+      <c r="G133" s="55"/>
+      <c r="H133" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="I133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B134" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="C134" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D134" s="57"/>
+      <c r="E134" s="57"/>
+      <c r="F134" s="57"/>
+      <c r="G134" s="57"/>
+      <c r="H134" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="I134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="B135" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="C135" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="D135" s="59"/>
+      <c r="E135" s="59"/>
+      <c r="F135" s="59"/>
+      <c r="G135" s="59"/>
+      <c r="H135" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="I135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="B136" s="57" t="s">
+        <v>273</v>
+      </c>
+      <c r="C136" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D136" s="57"/>
+      <c r="E136" s="57"/>
+      <c r="F136" s="57"/>
+      <c r="G136" s="57"/>
+      <c r="H136" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="B137" s="57" t="s">
+        <v>275</v>
+      </c>
+      <c r="C137" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D137" s="57"/>
+      <c r="E137" s="57"/>
+      <c r="F137" s="57">
+        <v>1</v>
+      </c>
+      <c r="G137" s="57"/>
+      <c r="H137" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="I137" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="B138" s="57" t="s">
+        <v>277</v>
+      </c>
+      <c r="C138" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D138" s="57"/>
+      <c r="E138" s="57"/>
+      <c r="F138" s="57"/>
+      <c r="G138" s="57"/>
+      <c r="H138" s="37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="B139" s="57" t="s">
+        <v>282</v>
+      </c>
+      <c r="C139" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D139" s="57"/>
+      <c r="E139" s="57">
+        <v>1</v>
+      </c>
+      <c r="F139" s="57"/>
+      <c r="G139" s="57"/>
+      <c r="H139" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="56" t="s">
+        <v>281</v>
+      </c>
+      <c r="B140" s="57" t="s">
+        <v>283</v>
+      </c>
+      <c r="C140" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D140" s="57"/>
+      <c r="E140" s="57">
+        <v>1</v>
+      </c>
+      <c r="F140" s="57"/>
+      <c r="G140" s="57"/>
+      <c r="H140" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="56" t="s">
+        <v>284</v>
+      </c>
+      <c r="B141" s="57" t="s">
+        <v>285</v>
+      </c>
+      <c r="C141" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D141" s="57"/>
+      <c r="E141" s="57">
+        <v>1</v>
+      </c>
+      <c r="F141" s="57"/>
+      <c r="G141" s="57"/>
+      <c r="H141" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B133" s="53" t="s">
+      <c r="B142" s="53" t="s">
         <v>176</v>
       </c>
-      <c r="C133" s="53" t="s">
+      <c r="C142" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="D133" s="53"/>
-      <c r="E133" s="53"/>
-      <c r="F133" s="53"/>
-      <c r="G133" s="53"/>
-      <c r="H133" s="53" t="s">
-        <v>124</v>
-      </c>
-      <c r="I133" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J133" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>Year</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A134" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="B134" s="55" t="s">
-        <v>233</v>
-      </c>
-      <c r="C134" s="55" t="s">
-        <v>145</v>
-      </c>
-      <c r="D134" s="55"/>
-      <c r="E134" s="55"/>
-      <c r="F134" s="55"/>
-      <c r="G134" s="55"/>
-      <c r="H134" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="I134" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J134" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>wu_rate</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="B135" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="C135" s="57" t="s">
-        <v>145</v>
-      </c>
-      <c r="D135" s="57"/>
-      <c r="E135" s="57"/>
-      <c r="F135" s="57"/>
-      <c r="G135" s="57"/>
-      <c r="H135" s="57" t="s">
-        <v>124</v>
-      </c>
-      <c r="I135" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J135" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>awuds_totw_cnt</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="B136" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="C136" s="59" t="s">
-        <v>145</v>
-      </c>
-      <c r="D136" s="59"/>
-      <c r="E136" s="59"/>
-      <c r="F136" s="59"/>
-      <c r="G136" s="59"/>
-      <c r="H136" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="I136" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="J136" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>awuds_dom_cnt</v>
+      <c r="D142" s="53"/>
+      <c r="E142" s="53"/>
+      <c r="F142" s="53"/>
+      <c r="G142" s="53"/>
+      <c r="H142" s="53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="52" t="s">
+        <v>279</v>
+      </c>
+      <c r="B143" s="53" t="s">
+        <v>279</v>
+      </c>
+      <c r="C143" s="53"/>
+      <c r="D143" s="53"/>
+      <c r="E143" s="53">
+        <v>1</v>
+      </c>
+      <c r="F143" s="53"/>
+      <c r="G143" s="53"/>
+      <c r="H143" s="53" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -5793,7 +4881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F149DC5D-F8E1-4049-87FC-CF29D8AE6CE9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
major update for databases, annual and monthly scripts, ..etc
</commit_message>
<xml_diff>
--- a/ml_experiments/annual_v_0_0/features_status.xlsx
+++ b/ml_experiments/annual_v_0_0/features_status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\water_use\CAWSC_WaterUse\ml_experiments\annual_v_0_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2131EFCE-A3D4-4C8F-8965-1CF72486FA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E344B319-EC91-476C-8BD1-701405FFCA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="288">
   <si>
     <t>is_swud</t>
   </si>
@@ -896,6 +896,12 @@
   </si>
   <si>
     <t>Monthly water use</t>
+  </si>
+  <si>
+    <t>avg_touris</t>
+  </si>
+  <si>
+    <t>Average Tourism</t>
   </si>
 </sst>
 </file>
@@ -1970,11 +1976,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:L144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="N144" sqref="N144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4868,6 +4874,17 @@
       <c r="G143" s="53"/>
       <c r="H143" s="53" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B144" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="H144" s="11" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>